<commit_message>
End of 6th Dec
</commit_message>
<xml_diff>
--- a/convolution_shape_calculator.xlsx
+++ b/convolution_shape_calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roryc\OneDrive - University College London\COMP0171 Bayesian Deep Learning\coursework-two\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C53B46-B666-4859-8D71-6710987AC612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425A020B-D12D-4D33-850C-D82C7587DDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{735C885E-D2A4-40D5-A563-4ED9510D86C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>input H</t>
   </si>
@@ -725,9 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FD2D92-0E7A-44F0-80DA-9F931EEF7ED2}">
   <dimension ref="B2:AG31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -898,7 +896,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" s="20">
         <v>2</v>
@@ -952,7 +950,7 @@
       </c>
       <c r="W7" s="10">
         <f>IF(E7&lt;&gt;"",E7,"")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X7" s="10">
         <f>IF(E7&lt;&gt;"",_xlfn.FLOOR.MATH(1+((C7+(2*M7)-(S7*(J7-1))-1)/G7)),"")</f>
@@ -968,11 +966,11 @@
       </c>
       <c r="AA7" s="10">
         <f>IF(E7&lt;&gt;"",W7*X7*Y7,"")</f>
-        <v>784</v>
+        <v>392</v>
       </c>
       <c r="AB7" s="10">
         <f>IF(E7&lt;&gt;"",W7*(B7/U7)*J7*K7+W7,"")</f>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="AC7" s="10" t="b">
         <f>IF(E7&lt;&gt;"",AND(MOD(B7,U7)=0,MOD(E7,U7)=0),"")</f>
@@ -987,15 +985,15 @@
       </c>
       <c r="AG7" s="7" t="str">
         <f>IF(E7&lt;&gt;"",_xlfn.CONCAT("nn.Conv2d(", B$6, " = ", B7, ", ",E$6, " = ", E7, ", ", F$6, " = ",F7, ", ", I$6," = ", I7, ", ",L$6," = ",L7,", ",R$6, " = ", R7, ", ", U$6, " = ", U7,")," ),"") &amp; IF(AF7="Yes",_xlfn.CONCAT(CHAR(10), "nn.ReLU(),"),"") &amp; IF(AE7="Yes",_xlfn.CONCAT(CHAR(10), "nn.BatchNorm2d(",W7,"),"),"")</f>
-        <v>nn.Conv2d(in_channels = 1, out_channels = 4, stride = 2, kernel_size = (3,2), padding = (1,0), dilation = 1, groups = 1),
+        <v>nn.Conv2d(in_channels = 1, out_channels = 2, stride = 2, kernel_size = (3,2), padding = (1,0), dilation = 1, groups = 1),
 nn.ReLU(),
-nn.BatchNorm2d(4),</v>
+nn.BatchNorm2d(2),</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B8" s="25">
         <f>W7</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="21">
         <f t="shared" ref="C8:C13" si="0">X7</f>
@@ -1006,7 +1004,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="21">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F8" s="21">
         <v>2</v>
@@ -1019,16 +1017,16 @@
         <f t="shared" ref="H8" si="3">IF(ISNUMBER(F8),F8,MID(F8, SEARCH(",", F8) + 1, SEARCH(")", F8) - SEARCH(",", F8) - 1))</f>
         <v>2</v>
       </c>
-      <c r="I8" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="21" t="str">
+      <c r="I8" s="21">
+        <v>3</v>
+      </c>
+      <c r="J8" s="21">
         <f t="shared" ref="J8:J13" si="4">IF(ISNUMBER(I8),I8,MID(I8, SEARCH("(", I8) + 1, SEARCH(",", I8) - SEARCH("(", I8) - 1))</f>
         <v>3</v>
       </c>
-      <c r="K8" s="21" t="str">
+      <c r="K8" s="21">
         <f t="shared" ref="K8" si="5">IF(ISNUMBER(I8),I8,MID(I8, SEARCH(",", I8) + 1, SEARCH(")", I8) - SEARCH(",", I8) - 1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L8" s="21" t="s">
         <v>28</v>
@@ -1060,7 +1058,7 @@
       </c>
       <c r="W8" s="11">
         <f>IF(E8&lt;&gt;"",E8,"")</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X8" s="11">
         <f>IF(E8&lt;&gt;"",_xlfn.FLOOR.MATH(1+((C8+(2*M8)-(S8*(J8-1))-1)/G8)),"")</f>
@@ -1068,39 +1066,42 @@
       </c>
       <c r="Y8" s="11">
         <f>IF(E8&lt;&gt;"",_xlfn.FLOOR.MATH(1+((D8+(2*N8)-(T8*(K8-1))-1)/H8)),"")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z8" s="11">
         <f>IF(E8&lt;&gt;"",B8*C8*D8,"")</f>
-        <v>784</v>
+        <v>392</v>
       </c>
       <c r="AA8" s="11">
         <f>IF(E8&lt;&gt;"",W8*X8*Y8,"")</f>
-        <v>392</v>
+        <v>168</v>
       </c>
       <c r="AB8" s="11">
         <f>IF(E8&lt;&gt;"",W8*(B8/U8)*J8*K8+W8,"")</f>
-        <v>200</v>
+        <v>76</v>
       </c>
       <c r="AC8" s="11" t="b">
         <f>IF(E8&lt;&gt;"",AND(MOD(B8,U8)=0,MOD(E8,U8)=0),"")</f>
         <v>1</v>
       </c>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="11"/>
+      <c r="AE8" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="AF8" s="11" t="s">
         <v>34</v>
       </c>
       <c r="AG8" s="8" t="str">
         <f t="shared" ref="AG8:AG13" si="10">IF(E8&lt;&gt;"",_xlfn.CONCAT("nn.Conv2d(", B$6, " = ", B8, ", ",E$6, " = ", E8, ", ", F$6, " = ",F8, ", ", I$6," = ", I8, ", ",L$6," = ",L8,", ",R$6, " = ", R8, ", ", U$6, " = ", U8,")," ),"") &amp; IF(AF8="Yes",_xlfn.CONCAT(CHAR(10), "nn.ReLU(),"),"") &amp; IF(AE8="Yes",_xlfn.CONCAT(CHAR(10), "nn.BatchNorm2d(",W8,"),"),"")</f>
-        <v>nn.Conv2d(in_channels = 4, out_channels = 8, stride = 2, kernel_size = (3,2), padding = (1,0), dilation = 1, groups = 1),
-nn.ReLU(),</v>
+        <v>nn.Conv2d(in_channels = 2, out_channels = 4, stride = 2, kernel_size = 3, padding = (1,0), dilation = 1, groups = 1),
+nn.ReLU(),
+nn.BatchNorm2d(4),</v>
       </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B9" s="22">
         <f t="shared" ref="B9:B13" si="11">W8</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9" s="22">
         <f t="shared" si="0"/>
@@ -1108,21 +1109,21 @@
       </c>
       <c r="D9" s="22">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="22">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F9" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="22">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="22">
         <f t="shared" ref="H9:H13" si="12">IF(ISNUMBER(F9),F9,MID(F9, SEARCH(",", F9) + 1, SEARCH(")", F9) - SEARCH(",", F9) - 1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="22">
         <v>3</v>
@@ -1135,57 +1136,57 @@
         <f t="shared" ref="K9:K13" si="13">IF(ISNUMBER(I9),I9,MID(I9, SEARCH(",", I9) + 1, SEARCH(")", I9) - SEARCH(",", I9) - 1))</f>
         <v>3</v>
       </c>
-      <c r="L9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="22" t="str">
+      <c r="L9" s="22">
+        <v>1</v>
+      </c>
+      <c r="M9" s="22">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="N9" s="22" t="str">
+      <c r="N9" s="22">
         <f t="shared" ref="N9:N13" si="14">IF(ISNUMBER(L9),L9,MID(L9, SEARCH(",", L9) + 1, SEARCH(")", L9) - SEARCH(",", L9) - 1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
       <c r="R9" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S9" s="22">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9" s="22">
         <f t="shared" ref="T9:T13" si="15">IF(ISNUMBER(R9),R9,MID(R9, SEARCH(",", R9) + 1, SEARCH(")", R9) - SEARCH(",", R9) - 1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9" s="22">
         <v>1</v>
       </c>
       <c r="W9" s="17">
         <f t="shared" ref="W9:W13" si="16">IF(E9&lt;&gt;"",E9,"")</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="X9" s="17">
         <f t="shared" ref="X9:X13" si="17">IF(E9&lt;&gt;"",_xlfn.FLOOR.MATH(1+((C9+(2*M9)-(S9*(J9-1))-1)/G9)),"")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="17">
         <f t="shared" ref="Y9:Y13" si="18">IF(E9&lt;&gt;"",_xlfn.FLOOR.MATH(1+((D9+(2*N9)-(T9*(K9-1))-1)/H9)),"")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Z9" s="17">
         <f t="shared" ref="Z9:Z13" si="19">IF(E9&lt;&gt;"",B9*C9*D9,"")</f>
-        <v>392</v>
+        <v>168</v>
       </c>
       <c r="AA9" s="17">
         <f t="shared" ref="AA9:AA13" si="20">IF(E9&lt;&gt;"",W9*X9*Y9,"")</f>
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="AB9" s="17">
         <f t="shared" ref="AB9:AB13" si="21">IF(E9&lt;&gt;"",W9*(B9/U9)*J9*K9+W9,"")</f>
-        <v>1168</v>
+        <v>296</v>
       </c>
       <c r="AC9" s="17" t="b">
         <f t="shared" ref="AC9:AC13" si="22">IF(E9&lt;&gt;"",AND(MOD(B9,U9)=0,MOD(E9,U9)=0),"")</f>
@@ -1200,23 +1201,23 @@
       </c>
       <c r="AG9" s="16" t="str">
         <f t="shared" si="10"/>
-        <v>nn.Conv2d(in_channels = 8, out_channels = 16, stride = 2, kernel_size = 3, padding = (1,0), dilation = 1, groups = 1),
+        <v>nn.Conv2d(in_channels = 4, out_channels = 8, stride = 1, kernel_size = 3, padding = 1, dilation = 2, groups = 1),
 nn.ReLU(),
-nn.BatchNorm2d(16),</v>
+nn.BatchNorm2d(8),</v>
       </c>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B10" s="22">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C10" s="22">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="22">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -1288,17 +1289,11 @@
         <v/>
       </c>
       <c r="AD10" s="1"/>
-      <c r="AE10" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF10" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
       <c r="AG10" s="16" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">
-nn.ReLU(),
-nn.BatchNorm2d(),</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.35">
@@ -1384,17 +1379,11 @@
         <v/>
       </c>
       <c r="AD11" s="1"/>
-      <c r="AE11" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF11" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
       <c r="AG11" s="16" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">
-nn.ReLU(),
-nn.BatchNorm2d(),</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.35">
@@ -1481,13 +1470,10 @@
       </c>
       <c r="AD12" s="1"/>
       <c r="AE12" s="17"/>
-      <c r="AF12" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="AF12" s="17"/>
       <c r="AG12" s="16" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">
-nn.ReLU(),</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.35">
@@ -1573,17 +1559,11 @@
         <v/>
       </c>
       <c r="AD13" s="1"/>
-      <c r="AE13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF13" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
       <c r="AG13" s="9" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">
-nn.ReLU(),
-nn.BatchNorm2d(),</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.35">
@@ -1680,7 +1660,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="6">
         <f>SUM(AB7:AB13)</f>
-        <v>1396</v>
+        <v>386</v>
       </c>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
@@ -1821,27 +1801,27 @@
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B21" s="20">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C21" s="20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D21" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F21" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="20">
         <f>IF(ISNUMBER(F21),F21,MID(F21, SEARCH("(", F21) + 1, SEARCH(",", F21) - SEARCH("(", F21) - 1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="20">
         <f>IF(ISNUMBER(F21),F21,MID(F21, SEARCH(",", F21) + 1, SEARCH(")", F21) - SEARCH(",", F21) - 1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21" s="20">
         <v>3</v>
@@ -1892,7 +1872,7 @@
       </c>
       <c r="W21" s="10">
         <f>IF(E21&lt;&gt;"",E21,"")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X21" s="10">
         <f>IF(E21&lt;&gt;"",G21*(C21-1)-(2*M21)+S21*(J21-1)+P21+1,"")</f>
@@ -1900,19 +1880,19 @@
       </c>
       <c r="Y21" s="10">
         <f>IF(E21&lt;&gt;"",H21*(D21-1)-(2*N21)+T21*(K21-1)+Q21+1,"")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z21" s="10">
         <f>IF(E21&lt;&gt;"",B21*C21*D21,"")</f>
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="AA21" s="10">
         <f>IF(E21&lt;&gt;"",W21*X21*Y21,"")</f>
-        <v>294</v>
+        <v>168</v>
       </c>
       <c r="AB21" s="10">
         <f>IF(E21&lt;&gt;"",(B21*(E21/U21)*J21*K21)+W21,"")</f>
-        <v>870</v>
+        <v>292</v>
       </c>
       <c r="AC21" s="10" t="b">
         <f>IF(E21&lt;&gt;"",AND(MOD(B21,U21)=0,MOD(E21,U21)=0),"")</f>
@@ -1926,15 +1906,15 @@
       </c>
       <c r="AG21" s="7" t="str">
         <f>IF(E21&lt;&gt;"",_xlfn.CONCAT("nn.ConvTranspose2d(",B$20," = ",B21,", ",E$20," = ",E21,", ",F$20," = ",F21,", ",I$20," = ",I21,", ",L$20," = ",L21,", ",O$20," = ",O21,", ",R$20," = ",R21,", ",U$20," = ",U21,"),"),"") &amp; IF(AF21="Yes",_xlfn.CONCAT(CHAR(10), "nn.ReLU(),"),"") &amp; IF(AE21="Yes",_xlfn.CONCAT(CHAR(10), "nn.BatchNorm2d(",W21,"),"),"")</f>
-        <v>nn.ConvTranspose2d(in_channels = 16, out_channels = 6, stride = 2, kernel_size = 3, padding = 0, output_padding = 0, dilation = 1, groups = 1),
+        <v>nn.ConvTranspose2d(in_channels = 8, out_channels = 4, stride = 1, kernel_size = 3, padding = 0, output_padding = 0, dilation = 1, groups = 1),
 nn.ReLU(),
-nn.BatchNorm2d(6),</v>
+nn.BatchNorm2d(4),</v>
       </c>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B22" s="27">
         <f>W21</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C22" s="24">
         <f t="shared" ref="C22:D22" si="34">X21</f>
@@ -1942,10 +1922,10 @@
       </c>
       <c r="D22" s="24">
         <f t="shared" si="34"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" s="24">
         <v>2</v>
@@ -1969,16 +1949,16 @@
         <f t="shared" ref="K22:K26" si="38">IF(ISNUMBER(I22),I22,MID(I22, SEARCH(",", I22) + 1, SEARCH(")", I22) - SEARCH(",", I22) - 1))</f>
         <v>3</v>
       </c>
-      <c r="L22" s="24">
-        <v>1</v>
-      </c>
-      <c r="M22" s="24">
+      <c r="L22" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="24" t="str">
         <f t="shared" ref="M22:M26" si="39">IF(ISNUMBER(L22),L22,MID(L22, SEARCH("(", L22) + 1, SEARCH(",", L22) - SEARCH("(", L22) - 1))</f>
         <v>1</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22" s="24" t="str">
         <f t="shared" ref="N22:N26" si="40">IF(ISNUMBER(L22),L22,MID(L22, SEARCH(",", L22) + 1, SEARCH(")", L22) - SEARCH(",", L22) - 1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" s="24">
         <v>1</v>
@@ -2007,7 +1987,7 @@
       </c>
       <c r="W22" s="19">
         <f t="shared" ref="W22:W28" si="45">IF(E22&lt;&gt;"",E22,"")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X22" s="19">
         <f t="shared" ref="X22:X28" si="46">IF(E22&lt;&gt;"",G22*(C22-1)-(2*M22)+S22*(J22-1)+P22+1,"")</f>
@@ -2019,34 +1999,37 @@
       </c>
       <c r="Z22" s="19">
         <f t="shared" ref="Z22:Z28" si="48">IF(E22&lt;&gt;"",B22*C22*D22,"")</f>
-        <v>294</v>
+        <v>168</v>
       </c>
       <c r="AA22" s="19">
         <f t="shared" ref="AA22:AA28" si="49">IF(E22&lt;&gt;"",W22*X22*Y22,"")</f>
-        <v>784</v>
+        <v>392</v>
       </c>
       <c r="AB22" s="19">
         <f t="shared" ref="AB22:AB28" si="50">IF(E22&lt;&gt;"",(B22*(E22/U22)*J22*K22)+W22,"")</f>
-        <v>220</v>
+        <v>74</v>
       </c>
       <c r="AC22" s="19" t="b">
         <f t="shared" ref="AC22:AC28" si="51">IF(E22&lt;&gt;"",AND(MOD(B22,U22)=0,MOD(E22,U22)=0),"")</f>
         <v>1</v>
       </c>
-      <c r="AE22" s="19"/>
+      <c r="AE22" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="AF22" s="19" t="s">
         <v>34</v>
       </c>
       <c r="AG22" s="18" t="str">
         <f t="shared" ref="AG22:AG28" si="52">IF(E22&lt;&gt;"",_xlfn.CONCAT("nn.ConvTranspose2d(",B$20," = ",B22,", ",E$20," = ",E22,", ",F$20," = ",F22,", ",I$20," = ",I22,", ",L$20," = ",L22,", ",O$20," = ",O22,", ",R$20," = ",R22,", ",U$20," = ",U22,"),"),"") &amp; IF(AF22="Yes",_xlfn.CONCAT(CHAR(10), "nn.ReLU(),"),"") &amp; IF(AE22="Yes",_xlfn.CONCAT(CHAR(10), "nn.BatchNorm2d(",W22,"),"),"")</f>
-        <v>nn.ConvTranspose2d(in_channels = 6, out_channels = 4, stride = 2, kernel_size = 3, padding = 1, output_padding = 1, dilation = 1, groups = 1),
-nn.ReLU(),</v>
+        <v>nn.ConvTranspose2d(in_channels = 4, out_channels = 2, stride = 2, kernel_size = 3, padding = (1,0), output_padding = 1, dilation = 1, groups = 1),
+nn.ReLU(),
+nn.BatchNorm2d(2),</v>
       </c>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B23" s="27">
         <f t="shared" ref="B23:B27" si="53">W22</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="24">
         <f t="shared" ref="C23:C27" si="54">X22</f>
@@ -2056,80 +2039,94 @@
         <f t="shared" ref="D23:D28" si="55">Y22</f>
         <v>14</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24" t="e">
+      <c r="E23" s="24">
+        <v>1</v>
+      </c>
+      <c r="F23" s="24">
+        <v>2</v>
+      </c>
+      <c r="G23" s="24">
         <f t="shared" si="35"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H23" s="24" t="e">
+        <v>2</v>
+      </c>
+      <c r="H23" s="24">
         <f t="shared" ref="H23:H26" si="56">IF(ISNUMBER(F23),F23,MID(F23, SEARCH(",", F23) + 1, SEARCH(")", F23) - SEARCH(",", F23) - 1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24" t="e">
+        <v>2</v>
+      </c>
+      <c r="I23" s="24">
+        <v>3</v>
+      </c>
+      <c r="J23" s="24">
         <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K23" s="24" t="e">
+        <v>3</v>
+      </c>
+      <c r="K23" s="24">
         <f t="shared" si="38"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24" t="e">
+        <v>3</v>
+      </c>
+      <c r="L23" s="24">
+        <v>1</v>
+      </c>
+      <c r="M23" s="24">
         <f t="shared" si="39"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N23" s="24" t="e">
+        <v>1</v>
+      </c>
+      <c r="N23" s="24">
         <f t="shared" si="40"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24" t="e">
+        <v>1</v>
+      </c>
+      <c r="O23" s="24">
+        <v>1</v>
+      </c>
+      <c r="P23" s="24">
         <f t="shared" si="41"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q23" s="24" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="24">
         <f t="shared" si="42"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24" t="e">
+        <v>1</v>
+      </c>
+      <c r="R23" s="24">
+        <v>1</v>
+      </c>
+      <c r="S23" s="24">
         <f t="shared" si="43"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T23" s="24" t="e">
+        <v>1</v>
+      </c>
+      <c r="T23" s="24">
         <f t="shared" si="44"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U23" s="24"/>
-      <c r="W23" s="19" t="str">
+        <v>1</v>
+      </c>
+      <c r="U23" s="24">
+        <v>1</v>
+      </c>
+      <c r="W23" s="19">
         <f t="shared" si="45"/>
-        <v/>
-      </c>
-      <c r="X23" s="19" t="str">
+        <v>1</v>
+      </c>
+      <c r="X23" s="19">
         <f t="shared" si="46"/>
-        <v/>
-      </c>
-      <c r="Y23" s="19" t="str">
+        <v>28</v>
+      </c>
+      <c r="Y23" s="19">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="Z23" s="19" t="str">
+        <v>28</v>
+      </c>
+      <c r="Z23" s="19">
         <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="AA23" s="19" t="str">
+        <v>392</v>
+      </c>
+      <c r="AA23" s="19">
         <f t="shared" si="49"/>
-        <v/>
-      </c>
-      <c r="AB23" s="19" t="str">
+        <v>784</v>
+      </c>
+      <c r="AB23" s="19">
         <f t="shared" si="50"/>
-        <v/>
-      </c>
-      <c r="AC23" s="19" t="str">
+        <v>19</v>
+      </c>
+      <c r="AC23" s="19" t="b">
         <f t="shared" si="51"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AE23" s="19" t="s">
         <v>34</v>
@@ -2139,23 +2136,23 @@
       </c>
       <c r="AG23" s="18" t="str">
         <f t="shared" si="52"/>
-        <v xml:space="preserve">
+        <v>nn.ConvTranspose2d(in_channels = 2, out_channels = 1, stride = 2, kernel_size = 3, padding = 1, output_padding = 1, dilation = 1, groups = 1),
 nn.ReLU(),
-nn.BatchNorm2d(),</v>
+nn.BatchNorm2d(1),</v>
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B24" s="27" t="str">
+      <c r="B24" s="27">
         <f t="shared" si="53"/>
-        <v/>
-      </c>
-      <c r="C24" s="24" t="str">
+        <v>1</v>
+      </c>
+      <c r="C24" s="24">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="D24" s="24" t="str">
+        <v>28</v>
+      </c>
+      <c r="D24" s="24">
         <f t="shared" si="55"/>
-        <v/>
+        <v>28</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
@@ -2232,17 +2229,11 @@
         <f t="shared" si="51"/>
         <v/>
       </c>
-      <c r="AE24" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF24" s="19" t="s">
-        <v>34</v>
-      </c>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
       <c r="AG24" s="18" t="str">
         <f t="shared" si="52"/>
-        <v xml:space="preserve">
-nn.ReLU(),
-nn.BatchNorm2d(),</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.35">
@@ -2334,13 +2325,10 @@
         <v/>
       </c>
       <c r="AE25" s="19"/>
-      <c r="AF25" s="19" t="s">
-        <v>34</v>
-      </c>
+      <c r="AF25" s="19"/>
       <c r="AG25" s="18" t="str">
         <f t="shared" si="52"/>
-        <v xml:space="preserve">
-nn.ReLU(),</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.35">
@@ -2630,7 +2618,7 @@
     <row r="31" spans="2:33" x14ac:dyDescent="0.35">
       <c r="AB31" s="6">
         <f>SUM(AB19:AB28)</f>
-        <v>1090</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>